<commit_message>
Maybe final in last month
</commit_message>
<xml_diff>
--- a/template Excel/HR/Employee.xlsx
+++ b/template Excel/HR/Employee.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ToolControlDatabase\template Excel\HR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2C0A98-08D1-43AF-AF03-74E77629FEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C96B91A-7AB4-49AB-A2B0-A109692181E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3961F9DE-4206-40BE-B32F-3CC7B35D6A5E}"/>
+    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="16440" xr2:uid="{3961F9DE-4206-40BE-B32F-3CC7B35D6A5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="84">
   <si>
     <t>HireDate</t>
   </si>
@@ -671,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CAB972D-657D-4C77-99C5-B859FDD68ABB}">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K51" sqref="K51"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2262,11 +2262,47 @@
         <v>39</v>
       </c>
     </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" s="1">
+        <v>35246</v>
+      </c>
+      <c r="D45" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" t="s">
+        <v>78</v>
+      </c>
+      <c r="F45">
+        <v>9</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H45">
+        <v>4</v>
+      </c>
+      <c r="I45" s="1">
+        <v>45527</v>
+      </c>
+      <c r="J45">
+        <v>1000</v>
+      </c>
+      <c r="K45" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G42" r:id="rId1" xr:uid="{4C6C4023-18A3-4E08-AC20-6C0C0B33A2E7}"/>
     <hyperlink ref="G43" r:id="rId2" xr:uid="{DA997B6D-FF52-492B-8691-B54A7BD54877}"/>
     <hyperlink ref="G44" r:id="rId3" xr:uid="{21FE4545-4380-4D6A-B328-F1212E927FAA}"/>
+    <hyperlink ref="G45" r:id="rId4" xr:uid="{07107982-E17F-4069-9B65-DAAA69F86DC1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>